<commit_message>
add new lua function
</commit_message>
<xml_diff>
--- a/Supplementary/文档/Lua脚本文档.xlsx
+++ b/Supplementary/文档/Lua脚本文档.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D71BF07-2B2E-457B-A3C9-9348CE135FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB1FCD1-9645-4399-86F6-967B28FE7CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{8CA9C43F-A422-443C-91EB-82DDAA2DCA05}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{8CA9C43F-A422-443C-91EB-82DDAA2DCA05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="797">
   <si>
     <t>iso_size()</t>
   </si>
@@ -12268,6 +12268,46 @@
   </si>
   <si>
     <t>game_path()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table&lt;int, table&lt;string, string&gt;&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_ordered_key_value_pairs(string section, [string load_from])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>获取</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>小节的有序键值对</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12573,7 +12613,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12582,10 +12622,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16791,8 +16831,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{95C8C70F-0A08-40EE-882E-F9E7CBD319C1}" name="表30" displayName="表30" ref="A231:C254" totalsRowShown="0" headerRowDxfId="148" dataDxfId="146" headerRowBorderDxfId="147" tableBorderDxfId="145">
-  <autoFilter ref="A231:C254" xr:uid="{95C8C70F-0A08-40EE-882E-F9E7CBD319C1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{95C8C70F-0A08-40EE-882E-F9E7CBD319C1}" name="表30" displayName="表30" ref="A231:C255" totalsRowShown="0" headerRowDxfId="148" dataDxfId="146" headerRowBorderDxfId="147" tableBorderDxfId="145">
+  <autoFilter ref="A231:C255" xr:uid="{95C8C70F-0A08-40EE-882E-F9E7CBD319C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -16807,8 +16847,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A625B1F9-0F50-4D0F-8C0A-5ED0E6B2DDF9}" name="表32" displayName="表32" ref="A256:C276" totalsRowShown="0" headerRowDxfId="141" dataDxfId="139" headerRowBorderDxfId="140">
-  <autoFilter ref="A256:C276" xr:uid="{A625B1F9-0F50-4D0F-8C0A-5ED0E6B2DDF9}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A625B1F9-0F50-4D0F-8C0A-5ED0E6B2DDF9}" name="表32" displayName="表32" ref="A257:C277" totalsRowShown="0" headerRowDxfId="141" dataDxfId="139" headerRowBorderDxfId="140">
+  <autoFilter ref="A257:C277" xr:uid="{A625B1F9-0F50-4D0F-8C0A-5ED0E6B2DDF9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -16839,7 +16879,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{27BF2D36-DEA5-4D7D-A02E-D1960B66BF3A}" name="表33" displayName="表33" ref="A281:C283" headerRowCount="0" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{27BF2D36-DEA5-4D7D-A02E-D1960B66BF3A}" name="表33" displayName="表33" ref="A282:C284" headerRowCount="0" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6EE63355-C87E-4E89-957B-33338EEBECA8}" name="列1" headerRowDxfId="132" dataDxfId="131"/>
     <tableColumn id="2" xr3:uid="{0371C133-76AF-4CE7-A076-F98E09274777}" name="列2" headerRowDxfId="130" dataDxfId="129"/>
@@ -16850,7 +16890,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{8FB12F79-BB88-42D0-83BD-F39A55B7E820}" name="表35" displayName="表35" ref="A285:C307" headerRowCount="0" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{8FB12F79-BB88-42D0-83BD-F39A55B7E820}" name="表35" displayName="表35" ref="A286:C308" headerRowCount="0" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F870DA49-FE02-4965-9BA2-C22DA388F93A}" name="列1" headerRowDxfId="124" dataDxfId="123"/>
     <tableColumn id="2" xr3:uid="{EDF4AD17-EFC3-4C50-9D98-69E7C9B397BD}" name="列2" headerRowDxfId="122" dataDxfId="121"/>
@@ -16861,7 +16901,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{E9766F59-B15E-4AD3-B3D7-262CE2928852}" name="表36" displayName="表36" ref="A308:C313" headerRowCount="0" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{E9766F59-B15E-4AD3-B3D7-262CE2928852}" name="表36" displayName="表36" ref="A309:C314" headerRowCount="0" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{66CF4FA4-633B-4807-9EB1-5660FC10D615}" name="列1" headerRowDxfId="116" dataDxfId="115"/>
     <tableColumn id="2" xr3:uid="{C9A87010-2F92-41C3-B254-5F9C97D11A53}" name="列2" headerRowDxfId="114" dataDxfId="113"/>
@@ -16872,7 +16912,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{250E9382-27E7-4D3C-8936-B3DAA52489C5}" name="表37" displayName="表37" ref="A315:C339" headerRowCount="0" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{250E9382-27E7-4D3C-8936-B3DAA52489C5}" name="表37" displayName="表37" ref="A316:C340" headerRowCount="0" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{67376287-A809-402E-9EE3-4A52F04A489A}" name="列1" headerRowDxfId="108" dataDxfId="107"/>
     <tableColumn id="2" xr3:uid="{C2A420D8-59DE-475C-A75B-E7A23356AD31}" name="列2" headerRowDxfId="106" dataDxfId="105"/>
@@ -16883,7 +16923,7 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{8115E9C9-98D1-4E31-BCB7-7C5CF91E154F}" name="表38" displayName="表38" ref="A340:C341" headerRowCount="0" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{8115E9C9-98D1-4E31-BCB7-7C5CF91E154F}" name="表38" displayName="表38" ref="A341:C342" headerRowCount="0" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A6DC2AF6-8D4E-470E-82E1-E4DBCFFEBCCA}" name="列1" headerRowDxfId="100" dataDxfId="99"/>
     <tableColumn id="2" xr3:uid="{16863727-9F7B-4D75-ACD3-6C34CB540888}" name="列2" headerRowDxfId="98" dataDxfId="97"/>
@@ -16894,7 +16934,7 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{E767F6D9-C0B7-42B4-A27E-818704055CB7}" name="表39" displayName="表39" ref="A343:C353" headerRowCount="0" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{E767F6D9-C0B7-42B4-A27E-818704055CB7}" name="表39" displayName="表39" ref="A344:C354" headerRowCount="0" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1E43DFEC-54F6-4A6E-AE01-0F8079E2B5DE}" name="列1" headerRowDxfId="92" dataDxfId="91"/>
     <tableColumn id="2" xr3:uid="{D21AEF5D-B438-4474-A662-A11B1B10C205}" name="列2" headerRowDxfId="90" dataDxfId="89"/>
@@ -16905,7 +16945,7 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{C3193565-D840-4B42-AFBF-D25127E0A2E5}" name="表40" displayName="表40" ref="A354:C355" headerRowCount="0" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{C3193565-D840-4B42-AFBF-D25127E0A2E5}" name="表40" displayName="表40" ref="A355:C356" headerRowCount="0" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C9CB15BD-7716-4ED5-BF07-FF95E006404C}" name="列1" headerRowDxfId="84" dataDxfId="83"/>
     <tableColumn id="2" xr3:uid="{F4F3EB43-F114-4535-AA32-D687E6D8B359}" name="列2" headerRowDxfId="82" dataDxfId="81"/>
@@ -16916,7 +16956,7 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{082D2DAE-A19A-4C09-A888-4F917C2E37E1}" name="表41" displayName="表41" ref="A357:C368" headerRowCount="0" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{082D2DAE-A19A-4C09-A888-4F917C2E37E1}" name="表41" displayName="表41" ref="A358:C369" headerRowCount="0" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A12B252F-D66B-4F1A-A738-89340EC8E765}" name="列1" headerRowDxfId="76" dataDxfId="75"/>
     <tableColumn id="2" xr3:uid="{2D4BA011-60EB-4554-9E50-E83EB5E0AA83}" name="列2" headerRowDxfId="74" dataDxfId="73"/>
@@ -16927,7 +16967,7 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{654F9517-D917-4876-8E8C-A4025B172B46}" name="表42" displayName="表42" ref="A369:C370" headerRowCount="0" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{654F9517-D917-4876-8E8C-A4025B172B46}" name="表42" displayName="表42" ref="A370:C371" headerRowCount="0" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{909B7F4F-7182-4190-9C36-1D92BD462FC0}" name="列1" headerRowDxfId="68" dataDxfId="67"/>
     <tableColumn id="2" xr3:uid="{7F230A7B-6862-4AB3-8B6D-77FDDA42A087}" name="列2" headerRowDxfId="66" dataDxfId="65"/>
@@ -16938,7 +16978,7 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{080910EA-FBD0-4BCC-8740-FB7D3ED8D3B8}" name="表43" displayName="表43" ref="A372:C411" headerRowCount="0" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{080910EA-FBD0-4BCC-8740-FB7D3ED8D3B8}" name="表43" displayName="表43" ref="A373:C412" headerRowCount="0" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{753B7110-5D54-4DBB-A3D8-31CEFCADDDA6}" name="列1" headerRowDxfId="60" dataDxfId="59"/>
     <tableColumn id="2" xr3:uid="{197B782B-ABDA-406D-86E0-2F9663F3E896}" name="列2" headerRowDxfId="58" dataDxfId="57"/>
@@ -16963,7 +17003,7 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{0438A464-C262-4416-AF51-6FAA386CAD4A}" name="表44" displayName="表44" ref="A412:C413" headerRowCount="0" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{0438A464-C262-4416-AF51-6FAA386CAD4A}" name="表44" displayName="表44" ref="A413:C414" headerRowCount="0" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B0573E76-7CDB-4A4D-9DE2-84DB8DE79DB8}" name="列1" headerRowDxfId="52" dataDxfId="51"/>
     <tableColumn id="2" xr3:uid="{2CB803CF-2E94-451E-B0A3-68C56EB18C1A}" name="列2" headerRowDxfId="50" dataDxfId="49"/>
@@ -17021,7 +17061,7 @@
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{08907876-9312-432F-8413-3E9465F0E0BE}" name="表5" displayName="表5" ref="A416:C421" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{08907876-9312-432F-8413-3E9465F0E0BE}" name="表5" displayName="表5" ref="A417:C422" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A0B12E05-DA5D-4F3C-AFAE-C976C301A6E1}" name="列1" headerRowDxfId="14" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{7539B8D2-C8AF-4692-9890-6E9EA428F9FE}" name="列2" headerRowDxfId="12" dataDxfId="11"/>
@@ -17430,10 +17470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF381881-FCB8-4D63-A433-CD8B5CF734B8}">
-  <dimension ref="A1:F421"/>
+  <dimension ref="A1:F422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.3"/>
@@ -17448,11 +17488,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -17774,11 +17814,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="21" t="s">
         <v>788</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
@@ -17859,11 +17899,11 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="21" t="s">
         <v>666</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
@@ -18168,11 +18208,11 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="24" t="s">
         <v>668</v>
       </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
@@ -19595,11 +19635,11 @@
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="24" t="s">
+      <c r="A173" s="21" t="s">
         <v>673</v>
       </c>
-      <c r="B173" s="24"/>
-      <c r="C173" s="24"/>
+      <c r="B173" s="21"/>
+      <c r="C173" s="21"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
     </row>
@@ -20516,7 +20556,7 @@
       <c r="B236" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="C236" s="3" t="s">
         <v>504</v>
       </c>
       <c r="D236" s="1"/>
@@ -20527,15 +20567,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="47" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>129</v>
+        <v>794</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>505</v>
+        <v>795</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>796</v>
       </c>
       <c r="D237" s="1"/>
       <c r="E237" s="2" t="s">
@@ -20545,15 +20585,15 @@
         <v>660</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="31" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="47" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E238" s="2" t="s">
         <v>121</v>
@@ -20564,13 +20604,13 @@
     </row>
     <row r="239" spans="1:6" ht="31" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E239" s="2" t="s">
         <v>122</v>
@@ -20581,13 +20621,13 @@
     </row>
     <row r="240" spans="1:6" ht="32" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E240" s="2" t="s">
         <v>662</v>
@@ -20598,24 +20638,24 @@
     </row>
     <row r="241" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="243" spans="1:5" ht="16" x14ac:dyDescent="0.3">
@@ -20623,23 +20663,23 @@
         <v>101</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D243" s="1"/>
       <c r="E243" s="1"/>
     </row>
     <row r="244" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D244" s="1"/>
       <c r="E244" s="1"/>
@@ -20649,10 +20689,10 @@
         <v>93</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D245" s="1"/>
       <c r="E245" s="1"/>
@@ -20662,62 +20702,62 @@
         <v>93</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D246" s="1"/>
       <c r="E246" s="1"/>
     </row>
-    <row r="247" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D247" s="1"/>
       <c r="E247" s="1"/>
     </row>
-    <row r="248" spans="1:5" ht="32" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D248" s="1"/>
       <c r="E248" s="1"/>
     </row>
     <row r="249" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D249" s="1"/>
       <c r="E249" s="1"/>
     </row>
-    <row r="250" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D250" s="1"/>
       <c r="E250" s="1"/>
@@ -20727,10 +20767,10 @@
         <v>93</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D251" s="1"/>
       <c r="E251" s="1"/>
@@ -20740,10 +20780,10 @@
         <v>93</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D252" s="1"/>
       <c r="E252" s="1"/>
@@ -20753,58 +20793,58 @@
         <v>93</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D253" s="1"/>
       <c r="E253" s="1"/>
     </row>
-    <row r="254" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D254" s="1"/>
       <c r="E254" s="1"/>
     </row>
     <row r="255" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="22" t="s">
-        <v>679</v>
-      </c>
-      <c r="B255" s="22"/>
-      <c r="C255" s="22"/>
+      <c r="A255" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>522</v>
+      </c>
       <c r="D255" s="1"/>
       <c r="E255" s="1"/>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A256" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B256" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C256" s="10" t="s">
-        <v>334</v>
-      </c>
+    <row r="256" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+      <c r="A256" s="22" t="s">
+        <v>679</v>
+      </c>
+      <c r="B256" s="22"/>
+      <c r="C256" s="22"/>
       <c r="D256" s="1"/>
       <c r="E256" s="1"/>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A257" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C257" s="2" t="s">
-        <v>523</v>
+      <c r="A257" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B257" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C257" s="10" t="s">
+        <v>334</v>
       </c>
       <c r="D257" s="1"/>
       <c r="E257" s="1"/>
@@ -20814,10 +20854,10 @@
         <v>101</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D258" s="1"/>
       <c r="E258" s="1"/>
@@ -20827,36 +20867,36 @@
         <v>101</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D259" s="1"/>
       <c r="E259" s="1"/>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="C260" s="18" t="s">
-        <v>762</v>
+        <v>155</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="D260" s="1"/>
       <c r="E260" s="1"/>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C261" s="2" t="s">
-        <v>526</v>
+        <v>761</v>
+      </c>
+      <c r="C261" s="18" t="s">
+        <v>762</v>
       </c>
       <c r="D261" s="1"/>
       <c r="E261" s="1"/>
@@ -20866,10 +20906,10 @@
         <v>101</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D262" s="1"/>
       <c r="E262" s="1"/>
@@ -20879,10 +20919,10 @@
         <v>101</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D263" s="1"/>
       <c r="E263" s="1"/>
@@ -20892,10 +20932,10 @@
         <v>101</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>767</v>
+        <v>528</v>
       </c>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
@@ -20905,10 +20945,10 @@
         <v>101</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>529</v>
+        <v>767</v>
       </c>
       <c r="D265" s="1"/>
       <c r="E265" s="1"/>
@@ -20918,10 +20958,10 @@
         <v>101</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D266" s="1"/>
       <c r="E266" s="1"/>
@@ -20931,88 +20971,88 @@
         <v>101</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D267" s="1"/>
       <c r="E267" s="1"/>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="C268" s="18" t="s">
-        <v>766</v>
+        <v>162</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>531</v>
       </c>
       <c r="D268" s="1"/>
       <c r="E268" s="1"/>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>532</v>
+        <v>765</v>
+      </c>
+      <c r="C269" s="18" t="s">
+        <v>766</v>
       </c>
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
     </row>
-    <row r="270" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D270" s="1"/>
       <c r="E270" s="1"/>
     </row>
-    <row r="271" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D271" s="1"/>
       <c r="E271" s="1"/>
     </row>
-    <row r="272" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D273" s="1"/>
       <c r="E273" s="1"/>
@@ -21022,106 +21062,106 @@
         <v>101</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>768</v>
+        <v>536</v>
       </c>
       <c r="D274" s="1"/>
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>692</v>
+        <v>101</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>693</v>
+        <v>166</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>694</v>
+        <v>768</v>
       </c>
       <c r="D275" s="1"/>
       <c r="E275" s="1"/>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D276" s="1"/>
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>695</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>698</v>
-      </c>
-      <c r="C277" s="3" t="s">
-        <v>699</v>
+        <v>696</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>697</v>
       </c>
       <c r="D277" s="1"/>
       <c r="E277" s="1"/>
     </row>
     <row r="278" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="22" t="s">
-        <v>680</v>
-      </c>
-      <c r="B278" s="22"/>
-      <c r="C278" s="22"/>
+      <c r="A278" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>699</v>
+      </c>
       <c r="D278" s="1"/>
       <c r="E278" s="1"/>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A279" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B279" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C279" s="10" t="s">
-        <v>334</v>
-      </c>
+    <row r="279" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+      <c r="A279" s="22" t="s">
+        <v>680</v>
+      </c>
+      <c r="B279" s="22"/>
+      <c r="C279" s="22"/>
       <c r="D279" s="1"/>
       <c r="E279" s="1"/>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A280" s="23" t="s">
-        <v>681</v>
-      </c>
-      <c r="B280" s="23"/>
-      <c r="C280" s="23"/>
+      <c r="A280" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B280" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C280" s="10" t="s">
+        <v>334</v>
+      </c>
       <c r="D280" s="1"/>
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="1:5" ht="16" x14ac:dyDescent="0.3">
-      <c r="A281" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B281" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C281" s="2" t="s">
-        <v>537</v>
-      </c>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A281" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="B281" s="23"/>
+      <c r="C281" s="23"/>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D282" s="1"/>
       <c r="E282" s="1"/>
@@ -21131,58 +21171,58 @@
         <v>170</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D283" s="1"/>
       <c r="E283" s="1"/>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A284" s="21" t="s">
-        <v>682</v>
-      </c>
-      <c r="B284" s="21"/>
-      <c r="C284" s="21"/>
+      <c r="A284" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>539</v>
+      </c>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
     </row>
-    <row r="285" spans="1:5" ht="32" x14ac:dyDescent="0.3">
-      <c r="A285" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C285" s="2" t="s">
-        <v>540</v>
-      </c>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A285" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="B285" s="25"/>
+      <c r="C285" s="25"/>
       <c r="D285" s="1"/>
       <c r="E285" s="1"/>
     </row>
-    <row r="286" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D286" s="1"/>
       <c r="E286" s="1"/>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>337</v>
+        <v>541</v>
       </c>
       <c r="D287" s="1"/>
       <c r="E287" s="1"/>
@@ -21192,49 +21232,49 @@
         <v>170</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>211</v>
+        <v>268</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>542</v>
+        <v>337</v>
       </c>
       <c r="D288" s="1"/>
       <c r="E288" s="1"/>
     </row>
-    <row r="289" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D289" s="1"/>
       <c r="E289" s="1"/>
     </row>
-    <row r="290" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D290" s="1"/>
       <c r="E290" s="1"/>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D291" s="1"/>
       <c r="E291" s="1"/>
@@ -21244,10 +21284,10 @@
         <v>174</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D292" s="1"/>
       <c r="E292" s="1"/>
@@ -21257,10 +21297,10 @@
         <v>174</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D293" s="1"/>
       <c r="E293" s="1"/>
@@ -21270,23 +21310,23 @@
         <v>174</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D294" s="1"/>
       <c r="E294" s="1"/>
     </row>
-    <row r="295" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D295" s="1"/>
       <c r="E295" s="1"/>
@@ -21296,36 +21336,36 @@
         <v>177</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D296" s="1"/>
       <c r="E296" s="1"/>
     </row>
-    <row r="297" spans="1:5" ht="48" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D297" s="1"/>
       <c r="E297" s="1"/>
     </row>
-    <row r="298" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D298" s="1"/>
       <c r="E298" s="1"/>
@@ -21335,49 +21375,49 @@
         <v>175</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D299" s="1"/>
       <c r="E299" s="1"/>
     </row>
-    <row r="300" spans="1:5" ht="32" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="C300" s="3" t="s">
-        <v>689</v>
+        <v>280</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>553</v>
       </c>
       <c r="D300" s="1"/>
       <c r="E300" s="1"/>
     </row>
-    <row r="301" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D301" s="1"/>
       <c r="E301" s="1"/>
     </row>
-    <row r="302" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C302" s="2" t="s">
-        <v>554</v>
+        <v>690</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>691</v>
       </c>
       <c r="D302" s="1"/>
       <c r="E302" s="1"/>
@@ -21387,10 +21427,10 @@
         <v>175</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D303" s="1"/>
       <c r="E303" s="1"/>
@@ -21400,62 +21440,62 @@
         <v>175</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>687</v>
+        <v>282</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D304" s="1"/>
       <c r="E304" s="1"/>
     </row>
-    <row r="305" spans="1:5" ht="32" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>283</v>
+        <v>687</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D305" s="1"/>
       <c r="E305" s="1"/>
     </row>
-    <row r="306" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D306" s="1"/>
       <c r="E306" s="1"/>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A307" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D307" s="1"/>
       <c r="E307" s="1"/>
     </row>
-    <row r="308" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D308" s="1"/>
       <c r="E308" s="1"/>
@@ -21465,36 +21505,36 @@
         <v>175</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D309" s="1"/>
       <c r="E309" s="1"/>
     </row>
-    <row r="310" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A310" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D310" s="1"/>
       <c r="E310" s="1"/>
     </row>
     <row r="311" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A311" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D311" s="1"/>
       <c r="E311" s="1"/>
@@ -21504,10 +21544,10 @@
         <v>175</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D312" s="1"/>
       <c r="E312" s="1"/>
@@ -21517,71 +21557,71 @@
         <v>175</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D313" s="1"/>
       <c r="E313" s="1"/>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A314" s="21" t="s">
-        <v>683</v>
-      </c>
-      <c r="B314" s="21"/>
-      <c r="C314" s="21"/>
+    <row r="314" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+      <c r="A314" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>565</v>
+      </c>
       <c r="D314" s="1"/>
       <c r="E314" s="1"/>
     </row>
-    <row r="315" spans="1:5" ht="32" x14ac:dyDescent="0.3">
-      <c r="A315" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B315" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>566</v>
-      </c>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A315" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="B315" s="25"/>
+      <c r="C315" s="25"/>
       <c r="D315" s="1"/>
       <c r="E315" s="1"/>
     </row>
-    <row r="316" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A316" s="2" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D316" s="1"/>
       <c r="E316" s="1"/>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A317" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>337</v>
+        <v>567</v>
       </c>
       <c r="D317" s="1"/>
       <c r="E317" s="1"/>
     </row>
-    <row r="318" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>568</v>
+        <v>337</v>
       </c>
       <c r="D318" s="1"/>
       <c r="E318" s="1"/>
@@ -21591,23 +21631,23 @@
         <v>170</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D319" s="1"/>
       <c r="E319" s="1"/>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A320" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>211</v>
+        <v>287</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>542</v>
+        <v>569</v>
       </c>
       <c r="D320" s="1"/>
       <c r="E320" s="1"/>
@@ -21617,10 +21657,10 @@
         <v>170</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>288</v>
+        <v>211</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>570</v>
+        <v>542</v>
       </c>
       <c r="D321" s="1"/>
       <c r="E321" s="1"/>
@@ -21630,10 +21670,10 @@
         <v>170</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D322" s="1"/>
       <c r="E322" s="1"/>
@@ -21643,62 +21683,62 @@
         <v>170</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D323" s="1"/>
       <c r="E323" s="1"/>
     </row>
-    <row r="324" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D324" s="1"/>
       <c r="E324" s="1"/>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D325" s="1"/>
       <c r="E325" s="1"/>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" s="2" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D326" s="1"/>
       <c r="E326" s="1"/>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D327" s="1"/>
       <c r="E327" s="1"/>
@@ -21708,10 +21748,10 @@
         <v>186</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D328" s="1"/>
       <c r="E328" s="1"/>
@@ -21721,23 +21761,23 @@
         <v>186</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D329" s="1"/>
       <c r="E329" s="1"/>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="2" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D330" s="1"/>
       <c r="E330" s="1"/>
@@ -21747,10 +21787,10 @@
         <v>174</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D331" s="1"/>
       <c r="E331" s="1"/>
@@ -21760,10 +21800,10 @@
         <v>174</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D332" s="1"/>
       <c r="E332" s="1"/>
@@ -21773,10 +21813,10 @@
         <v>174</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D333" s="1"/>
       <c r="E333" s="1"/>
@@ -21786,36 +21826,36 @@
         <v>174</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D334" s="1"/>
       <c r="E334" s="1"/>
     </row>
-    <row r="335" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D335" s="1"/>
       <c r="E335" s="1"/>
     </row>
     <row r="336" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A336" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>687</v>
+        <v>299</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D336" s="1"/>
       <c r="E336" s="1"/>
@@ -21825,10 +21865,10 @@
         <v>175</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>283</v>
+        <v>687</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D337" s="1"/>
       <c r="E337" s="1"/>
@@ -21838,10 +21878,10 @@
         <v>175</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D338" s="1"/>
       <c r="E338" s="1"/>
@@ -21851,10 +21891,10 @@
         <v>175</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C339" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D339" s="1"/>
       <c r="E339" s="1"/>
@@ -21864,84 +21904,84 @@
         <v>175</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>188</v>
+        <v>284</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D340" s="1"/>
       <c r="E340" s="1"/>
     </row>
     <row r="341" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A341" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D341" s="1"/>
       <c r="E341" s="1"/>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A342" s="21" t="s">
-        <v>684</v>
-      </c>
-      <c r="B342" s="21"/>
-      <c r="C342" s="21"/>
+    <row r="342" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+      <c r="A342" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>590</v>
+      </c>
       <c r="D342" s="1"/>
       <c r="E342" s="1"/>
     </row>
-    <row r="343" spans="1:5" ht="32" x14ac:dyDescent="0.3">
-      <c r="A343" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B343" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C343" s="2" t="s">
-        <v>591</v>
-      </c>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A343" s="25" t="s">
+        <v>684</v>
+      </c>
+      <c r="B343" s="25"/>
+      <c r="C343" s="25"/>
       <c r="D343" s="1"/>
       <c r="E343" s="1"/>
     </row>
-    <row r="344" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A344" s="2" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D344" s="1"/>
       <c r="E344" s="1"/>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A345" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>337</v>
+        <v>592</v>
       </c>
       <c r="D345" s="1"/>
       <c r="E345" s="1"/>
     </row>
-    <row r="346" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>593</v>
+        <v>337</v>
       </c>
       <c r="D346" s="1"/>
       <c r="E346" s="1"/>
@@ -21951,23 +21991,23 @@
         <v>185</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D347" s="1"/>
       <c r="E347" s="1"/>
     </row>
-    <row r="348" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A348" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D348" s="1"/>
       <c r="E348" s="1"/>
@@ -21977,10 +22017,10 @@
         <v>175</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D349" s="1"/>
       <c r="E349" s="1"/>
@@ -21990,10 +22030,10 @@
         <v>175</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D350" s="1"/>
       <c r="E350" s="1"/>
@@ -22003,10 +22043,10 @@
         <v>175</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D351" s="1"/>
       <c r="E351" s="1"/>
@@ -22016,97 +22056,97 @@
         <v>175</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C352" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D352" s="1"/>
       <c r="E352" s="1"/>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A353" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D353" s="1"/>
       <c r="E353" s="1"/>
     </row>
-    <row r="354" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>192</v>
+        <v>284</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D354" s="1"/>
       <c r="E354" s="1"/>
     </row>
     <row r="355" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A355" s="2" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D355" s="1"/>
       <c r="E355" s="1"/>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A356" s="21" t="s">
-        <v>685</v>
-      </c>
-      <c r="B356" s="21"/>
-      <c r="C356" s="21"/>
+    <row r="356" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+      <c r="A356" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>602</v>
+      </c>
       <c r="D356" s="1"/>
       <c r="E356" s="1"/>
     </row>
-    <row r="357" spans="1:5" ht="32" x14ac:dyDescent="0.3">
-      <c r="A357" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B357" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C357" s="2" t="s">
-        <v>603</v>
-      </c>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A357" s="25" t="s">
+        <v>685</v>
+      </c>
+      <c r="B357" s="25"/>
+      <c r="C357" s="25"/>
       <c r="D357" s="1"/>
       <c r="E357" s="1"/>
     </row>
-    <row r="358" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A358" s="2" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D358" s="1"/>
       <c r="E358" s="1"/>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A359" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>337</v>
+        <v>604</v>
       </c>
       <c r="D359" s="1"/>
       <c r="E359" s="1"/>
@@ -22116,49 +22156,49 @@
         <v>170</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>219</v>
+        <v>268</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>605</v>
+        <v>337</v>
       </c>
       <c r="D360" s="1"/>
       <c r="E360" s="1"/>
     </row>
-    <row r="361" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>303</v>
+        <v>219</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D361" s="1"/>
       <c r="E361" s="1"/>
     </row>
     <row r="362" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A362" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C362" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D362" s="1"/>
       <c r="E362" s="1"/>
     </row>
-    <row r="363" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A363" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D363" s="1"/>
       <c r="E363" s="1"/>
@@ -22168,10 +22208,10 @@
         <v>175</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D364" s="1"/>
       <c r="E364" s="1"/>
@@ -22181,10 +22221,10 @@
         <v>175</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D365" s="1"/>
       <c r="E365" s="1"/>
@@ -22194,10 +22234,10 @@
         <v>175</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D366" s="1"/>
       <c r="E366" s="1"/>
@@ -22207,97 +22247,97 @@
         <v>175</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D367" s="1"/>
       <c r="E367" s="1"/>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A368" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C368" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D368" s="1"/>
       <c r="E368" s="1"/>
     </row>
-    <row r="369" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>196</v>
+        <v>284</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D369" s="1"/>
       <c r="E369" s="1"/>
     </row>
     <row r="370" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A370" s="2" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C370" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D370" s="1"/>
       <c r="E370" s="1"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A371" s="21" t="s">
-        <v>686</v>
-      </c>
-      <c r="B371" s="21"/>
-      <c r="C371" s="21"/>
+    <row r="371" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+      <c r="A371" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>615</v>
+      </c>
       <c r="D371" s="1"/>
       <c r="E371" s="1"/>
     </row>
-    <row r="372" spans="1:5" ht="32" x14ac:dyDescent="0.3">
-      <c r="A372" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B372" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C372" s="2" t="s">
-        <v>616</v>
-      </c>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A372" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="B372" s="25"/>
+      <c r="C372" s="25"/>
       <c r="D372" s="1"/>
       <c r="E372" s="1"/>
     </row>
-    <row r="373" spans="1:5" ht="31" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" ht="32" x14ac:dyDescent="0.3">
       <c r="A373" s="2" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D373" s="1"/>
       <c r="E373" s="1"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" ht="31" x14ac:dyDescent="0.3">
       <c r="A374" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>337</v>
+        <v>617</v>
       </c>
       <c r="D374" s="1"/>
       <c r="E374" s="1"/>
@@ -22307,23 +22347,23 @@
         <v>170</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>211</v>
+        <v>268</v>
       </c>
       <c r="C375" s="2" t="s">
-        <v>618</v>
+        <v>337</v>
       </c>
       <c r="D375" s="1"/>
       <c r="E375" s="1"/>
     </row>
-    <row r="376" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D376" s="1"/>
       <c r="E376" s="1"/>
@@ -22333,10 +22373,10 @@
         <v>170</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D377" s="1"/>
       <c r="E377" s="1"/>
@@ -22346,23 +22386,23 @@
         <v>170</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D378" s="1"/>
       <c r="E378" s="1"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A379" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>307</v>
+        <v>169</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D379" s="1"/>
       <c r="E379" s="1"/>
@@ -22372,10 +22412,10 @@
         <v>170</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D380" s="1"/>
       <c r="E380" s="1"/>
@@ -22385,10 +22425,10 @@
         <v>170</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D381" s="1"/>
       <c r="E381" s="1"/>
@@ -22398,10 +22438,10 @@
         <v>170</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C382" s="2" t="s">
-        <v>570</v>
+        <v>624</v>
       </c>
       <c r="D382" s="1"/>
       <c r="E382" s="1"/>
@@ -22411,10 +22451,10 @@
         <v>170</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C383" s="2" t="s">
-        <v>625</v>
+        <v>570</v>
       </c>
       <c r="D383" s="1"/>
       <c r="E383" s="1"/>
@@ -22424,10 +22464,10 @@
         <v>170</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>219</v>
+        <v>311</v>
       </c>
       <c r="C384" s="2" t="s">
-        <v>605</v>
+        <v>625</v>
       </c>
       <c r="D384" s="1"/>
       <c r="E384" s="1"/>
@@ -22437,10 +22477,10 @@
         <v>170</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="C385" s="2" t="s">
-        <v>626</v>
+        <v>605</v>
       </c>
       <c r="D385" s="1"/>
       <c r="E385" s="1"/>
@@ -22450,23 +22490,23 @@
         <v>170</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>312</v>
+        <v>245</v>
       </c>
       <c r="C386" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D386" s="1"/>
       <c r="E386" s="1"/>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D387" s="1"/>
       <c r="E387" s="1"/>
@@ -22476,10 +22516,10 @@
         <v>174</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D388" s="1"/>
       <c r="E388" s="1"/>
@@ -22489,10 +22529,10 @@
         <v>174</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D389" s="1"/>
       <c r="E389" s="1"/>
@@ -22502,10 +22542,10 @@
         <v>174</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C390" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D390" s="1"/>
       <c r="E390" s="1"/>
@@ -22515,10 +22555,10 @@
         <v>174</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D391" s="1"/>
       <c r="E391" s="1"/>
@@ -22528,10 +22568,10 @@
         <v>174</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C392" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D392" s="1"/>
       <c r="E392" s="1"/>
@@ -22541,10 +22581,10 @@
         <v>174</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C393" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D393" s="1"/>
       <c r="E393" s="1"/>
@@ -22554,10 +22594,10 @@
         <v>174</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C394" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D394" s="1"/>
       <c r="E394" s="1"/>
@@ -22567,10 +22607,10 @@
         <v>174</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C395" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D395" s="1"/>
       <c r="E395" s="1"/>
@@ -22580,10 +22620,10 @@
         <v>174</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C396" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D396" s="1"/>
       <c r="E396" s="1"/>
@@ -22593,10 +22633,10 @@
         <v>174</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C397" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D397" s="1"/>
       <c r="E397" s="1"/>
@@ -22606,10 +22646,10 @@
         <v>174</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C398" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D398" s="1"/>
       <c r="E398" s="1"/>
@@ -22619,10 +22659,10 @@
         <v>174</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C399" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D399" s="1"/>
       <c r="E399" s="1"/>
@@ -22632,10 +22672,10 @@
         <v>174</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C400" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D400" s="1"/>
       <c r="E400" s="1"/>
@@ -22645,10 +22685,10 @@
         <v>174</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C401" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D401" s="1"/>
       <c r="E401" s="1"/>
@@ -22658,10 +22698,10 @@
         <v>174</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C402" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D402" s="1"/>
       <c r="E402" s="1"/>
@@ -22671,10 +22711,10 @@
         <v>174</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>298</v>
+        <v>328</v>
       </c>
       <c r="C403" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D403" s="1"/>
       <c r="E403" s="1"/>
@@ -22684,10 +22724,10 @@
         <v>174</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="C404" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D404" s="1"/>
       <c r="E404" s="1"/>
@@ -22697,10 +22737,10 @@
         <v>174</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D405" s="1"/>
       <c r="E405" s="1"/>
@@ -22710,10 +22750,10 @@
         <v>174</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D406" s="1"/>
       <c r="E406" s="1"/>
@@ -22723,23 +22763,23 @@
         <v>174</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C407" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D407" s="1"/>
       <c r="E407" s="1"/>
     </row>
-    <row r="408" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>300</v>
+        <v>332</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D408" s="1"/>
       <c r="E408" s="1"/>
@@ -22749,10 +22789,10 @@
         <v>175</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D409" s="1"/>
       <c r="E409" s="1"/>
@@ -22762,72 +22802,72 @@
         <v>175</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C410" s="2" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A411" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C411" s="2" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="412" spans="1:5" ht="16" x14ac:dyDescent="0.3">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="413" spans="1:5" ht="16" x14ac:dyDescent="0.3">
       <c r="A413" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B413" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C413" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A414" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B413" s="2" t="s">
+      <c r="B414" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C413" s="2" t="s">
+      <c r="C414" s="2" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="414" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A414" s="22" t="s">
+    <row r="415" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+      <c r="A415" s="22" t="s">
         <v>747</v>
       </c>
-      <c r="B414" s="22"/>
-      <c r="C414" s="22"/>
-    </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A415" s="15" t="s">
+      <c r="B415" s="22"/>
+      <c r="C415" s="22"/>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A416" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="B415" s="16" t="s">
+      <c r="B416" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="C415" s="17" t="s">
+      <c r="C416" s="17" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="416" spans="1:5" ht="16" x14ac:dyDescent="0.3">
-      <c r="A416" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B416" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="C416" s="3" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="16" x14ac:dyDescent="0.3">
@@ -22835,21 +22875,21 @@
         <v>25</v>
       </c>
       <c r="B417" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="C417" s="3" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" ht="16" x14ac:dyDescent="0.3">
+      <c r="A418" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B418" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C417" s="19" t="s">
+      <c r="C418" s="19" t="s">
         <v>753</v>
-      </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A418" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B418" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="C418" s="18" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
@@ -22857,38 +22897,56 @@
         <v>29</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="C419" s="14" t="s">
-        <v>755</v>
+        <v>748</v>
+      </c>
+      <c r="C419" s="18" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" s="2" t="s">
-        <v>756</v>
+        <v>29</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C420" s="14" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="B421" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C421" s="14" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A422" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B421" s="2" t="s">
+      <c r="B422" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="C421" s="18" t="s">
+      <c r="C422" s="18" t="s">
         <v>759</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A357:C357"/>
+    <mergeCell ref="A372:C372"/>
+    <mergeCell ref="A256:C256"/>
+    <mergeCell ref="A279:C279"/>
+    <mergeCell ref="A281:C281"/>
+    <mergeCell ref="A285:C285"/>
+    <mergeCell ref="A315:C315"/>
     <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A414:C414"/>
+    <mergeCell ref="A415:C415"/>
     <mergeCell ref="A121:C121"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A39:C39"/>
@@ -22902,14 +22960,7 @@
     <mergeCell ref="A175:C175"/>
     <mergeCell ref="A207:C207"/>
     <mergeCell ref="A230:C230"/>
-    <mergeCell ref="A342:C342"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A371:C371"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="A278:C278"/>
-    <mergeCell ref="A280:C280"/>
-    <mergeCell ref="A284:C284"/>
-    <mergeCell ref="A314:C314"/>
+    <mergeCell ref="A343:C343"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>